<commit_message>
4 sticky notes to go
</commit_message>
<xml_diff>
--- a/Relevant Documents/LOOCV_details.xlsx
+++ b/Relevant Documents/LOOCV_details.xlsx
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,67 +616,64 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D33" si="0">IF(B2=C2,1,0)</f>
-        <v>1</v>
+        <f>IF(B2=C2,1,0)</f>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H2">
         <f>SUM(D2:D30)/COUNTIF(E:E,"=0")*100</f>
-        <v>62.068965517241381</v>
+        <v>20.689655172413794</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
+        <f>IF(B3=C3,1,0)</f>
         <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>78</v>
       </c>
       <c r="H3">
         <f>SUM(D31:D68)/COUNTIF(E:E,"=1")*100</f>
-        <v>68.421052631578945</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(B4=C4,1,0)</f>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -684,16 +681,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f>IF(B5=C5,1,0)</f>
         <v>0</v>
       </c>
       <c r="E5">
@@ -702,17 +699,17 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(B6=C6,1,0)</f>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -720,17 +717,17 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(B7=C7,1,0)</f>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -738,17 +735,17 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(B8=C8,1,0)</f>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -756,16 +753,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f>IF(B9=C9,1,0)</f>
         <v>0</v>
       </c>
       <c r="E9">
@@ -774,7 +771,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -783,7 +780,7 @@
         <v>21</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f>IF(B10=C10,1,0)</f>
         <v>0</v>
       </c>
       <c r="E10">
@@ -792,17 +789,17 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(B11=C11,1,0)</f>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -810,17 +807,17 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(B12=C12,1,0)</f>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -828,61 +825,61 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f>IF(B13=C13,1,0)</f>
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f>IF(B14=C14,1,0)</f>
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(B15=C15,1,0)</f>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -891,119 +888,119 @@
         <v>3</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f>IF(B16=C16,1,0)</f>
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(B17=C17,1,0)</f>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(B18=C18,1,0)</f>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f>IF(B19=C19,1,0)</f>
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(B20=C20,1,0)</f>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(B21=C21,1,0)</f>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f>IF(B22=C22,1,0)</f>
         <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" t="s">
         <v>74</v>
@@ -1011,104 +1008,107 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>IF(B23=C23,1,0)</f>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" t="s">
         <v>1</v>
       </c>
       <c r="L23">
         <f>COUNTIF(C$2:C$30,K23)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M23">
         <f>L23/$L$29*100</f>
-        <v>33.333333333333329</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f>IF(B24=C24,1,0)</f>
         <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" t="s">
         <v>3</v>
       </c>
       <c r="L24">
-        <f t="shared" ref="L24:L28" si="1">COUNTIF(C$2:C$30,K24)</f>
+        <f t="shared" ref="L24:L27" si="0">COUNTIF(C$2:C$30,K24)</f>
         <v>8</v>
       </c>
       <c r="M24">
-        <f t="shared" ref="M24:M28" si="2">L24/$L$29*100</f>
+        <f t="shared" ref="M24:M28" si="1">L24/$L$29*100</f>
         <v>26.666666666666668</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f>IF(B25=C25,1,0)</f>
         <v>1</v>
       </c>
       <c r="E25">
         <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>77</v>
       </c>
       <c r="K25" t="s">
         <v>5</v>
       </c>
       <c r="L25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M25">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="2"/>
         <v>16.666666666666664</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(B26=C26,1,0)</f>
+        <v>1</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1117,26 +1117,26 @@
         <v>21</v>
       </c>
       <c r="L26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M26">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="2"/>
-        <v>13.333333333333334</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f>IF(B27=C27,1,0)</f>
         <v>1</v>
       </c>
       <c r="E27">
@@ -1146,26 +1146,26 @@
         <v>8</v>
       </c>
       <c r="L27">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M27">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="2"/>
-        <v>6.666666666666667</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f>IF(B28=C28,1,0)</f>
         <v>1</v>
       </c>
       <c r="E28">
@@ -1178,22 +1178,22 @@
         <v>1</v>
       </c>
       <c r="M28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f>IF(B29=C29,1,0)</f>
         <v>1</v>
       </c>
       <c r="E29">
@@ -1206,16 +1206,16 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f>IF(B30=C30,1,0)</f>
         <v>1</v>
       </c>
       <c r="E30">
@@ -1224,43 +1224,43 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(B31=C31,1,0)</f>
+        <v>1</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f>IF(B32=C32,1,0)</f>
         <v>1</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
         <v>1</v>
@@ -1269,34 +1269,34 @@
         <v>1</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f>IF(B33=C33,1,0)</f>
         <v>1</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:D65" si="3">IF(B34=C34,1,0)</f>
+        <f>IF(B34=C34,1,0)</f>
         <v>1</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
@@ -1305,11 +1305,11 @@
         <v>1</v>
       </c>
       <c r="D35">
-        <f t="shared" si="3"/>
+        <f>IF(B35=C35,1,0)</f>
         <v>1</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35" t="s">
         <v>76</v>
@@ -1317,7 +1317,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
@@ -1326,143 +1326,143 @@
         <v>1</v>
       </c>
       <c r="D36">
-        <f t="shared" si="3"/>
+        <f>IF(B36=C36,1,0)</f>
         <v>1</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36" t="s">
         <v>1</v>
       </c>
       <c r="L36">
         <f>COUNTIF(C$31:C$68,K36)</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="M36">
         <f>L36/$L$42*100</f>
-        <v>51.282051282051277</v>
+        <v>61.53846153846154</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D37">
-        <f t="shared" si="3"/>
+        <f>IF(B37=C37,1,0)</f>
         <v>1</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" t="s">
         <v>3</v>
       </c>
       <c r="L37">
-        <f t="shared" ref="L37:L41" si="4">COUNTIF(C$31:C$68,K37)</f>
+        <f t="shared" ref="L37:L40" si="2">COUNTIF(C$31:C$68,K37)</f>
         <v>9</v>
       </c>
       <c r="M37">
-        <f t="shared" ref="M37:M41" si="5">L37/$L$42*100</f>
+        <f t="shared" ref="M37:M41" si="3">L37/$L$42*100</f>
         <v>23.076923076923077</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D38">
-        <f t="shared" si="3"/>
+        <f>IF(B38=C38,1,0)</f>
         <v>1</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K38" t="s">
         <v>5</v>
       </c>
       <c r="L38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="M38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>7.6923076923076925</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D39">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(B39=C39,1,0)</f>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39" t="s">
         <v>21</v>
       </c>
       <c r="L39">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="M39">
-        <f t="shared" si="5"/>
-        <v>7.6923076923076925</v>
+        <f t="shared" si="3"/>
+        <v>2.5641025641025639</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D40">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(B40=C40,1,0)</f>
+        <v>1</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40" t="s">
         <v>8</v>
       </c>
       <c r="L40">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="M40">
-        <f t="shared" si="5"/>
-        <v>7.6923076923076925</v>
+        <f t="shared" si="3"/>
+        <v>2.5641025641025639</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
@@ -1471,11 +1471,11 @@
         <v>1</v>
       </c>
       <c r="D41">
-        <f t="shared" si="3"/>
+        <f>IF(B41=C41,1,0)</f>
         <v>1</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41" t="s">
         <v>79</v>
@@ -1485,26 +1485,26 @@
         <v>1</v>
       </c>
       <c r="M41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2.5641025641025639</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D42">
-        <f t="shared" si="3"/>
+        <f>IF(B42=C42,1,0)</f>
         <v>1</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L42">
         <f>SUM(L36:L41)</f>
@@ -1513,16 +1513,16 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D43">
-        <f t="shared" si="3"/>
+        <f>IF(B43=C43,1,0)</f>
         <v>1</v>
       </c>
       <c r="E43">
@@ -1531,7 +1531,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
@@ -1540,7 +1540,7 @@
         <v>1</v>
       </c>
       <c r="D44">
-        <f t="shared" si="3"/>
+        <f>IF(B44=C44,1,0)</f>
         <v>1</v>
       </c>
       <c r="E44">
@@ -1549,7 +1549,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B45" t="s">
         <v>1</v>
@@ -1558,7 +1558,7 @@
         <v>1</v>
       </c>
       <c r="D45">
-        <f t="shared" si="3"/>
+        <f>IF(B45=C45,1,0)</f>
         <v>1</v>
       </c>
       <c r="E45">
@@ -1567,7 +1567,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
@@ -1576,7 +1576,7 @@
         <v>1</v>
       </c>
       <c r="D46">
-        <f t="shared" si="3"/>
+        <f>IF(B46=C46,1,0)</f>
         <v>1</v>
       </c>
       <c r="E46">
@@ -1585,17 +1585,17 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B47" t="s">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(B47=C47,1,0)</f>
+        <v>1</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -1603,7 +1603,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B48" t="s">
         <v>1</v>
@@ -1612,7 +1612,7 @@
         <v>1</v>
       </c>
       <c r="D48">
-        <f t="shared" si="3"/>
+        <f>IF(B48=C48,1,0)</f>
         <v>1</v>
       </c>
       <c r="E48">
@@ -1621,16 +1621,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D49">
-        <f t="shared" si="3"/>
+        <f>IF(B49=C49,1,0)</f>
         <v>1</v>
       </c>
       <c r="E49">
@@ -1639,7 +1639,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
@@ -1648,7 +1648,7 @@
         <v>1</v>
       </c>
       <c r="D50">
-        <f t="shared" si="3"/>
+        <f>IF(B50=C50,1,0)</f>
         <v>1</v>
       </c>
       <c r="E50">
@@ -1657,17 +1657,17 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B51" t="s">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(B51=C51,1,0)</f>
+        <v>1</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -1675,17 +1675,17 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D52">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(B52=C52,1,0)</f>
+        <v>1</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -1693,17 +1693,17 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D53">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(B53=C53,1,0)</f>
+        <v>1</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B54" t="s">
         <v>1</v>
@@ -1720,7 +1720,7 @@
         <v>1</v>
       </c>
       <c r="D54">
-        <f t="shared" si="3"/>
+        <f>IF(B54=C54,1,0)</f>
         <v>1</v>
       </c>
       <c r="E54">
@@ -1729,16 +1729,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D55">
-        <f t="shared" si="3"/>
+        <f>IF(B55=C55,1,0)</f>
         <v>1</v>
       </c>
       <c r="E55">
@@ -1747,17 +1747,17 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D56">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(B56=C56,1,0)</f>
+        <v>1</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -1765,16 +1765,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B57" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D57">
-        <f t="shared" si="3"/>
+        <f>IF(B57=C57,1,0)</f>
         <v>1</v>
       </c>
       <c r="E57">
@@ -1783,16 +1783,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D58">
-        <f t="shared" si="3"/>
+        <f>IF(B58=C58,1,0)</f>
         <v>1</v>
       </c>
       <c r="E58">
@@ -1801,7 +1801,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B59" t="s">
         <v>1</v>
@@ -1810,7 +1810,7 @@
         <v>1</v>
       </c>
       <c r="D59">
-        <f t="shared" si="3"/>
+        <f>IF(B59=C59,1,0)</f>
         <v>1</v>
       </c>
       <c r="E59">
@@ -1819,17 +1819,17 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B60" t="s">
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D60">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(B60=C60,1,0)</f>
+        <v>1</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -1837,7 +1837,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B61" t="s">
         <v>1</v>
@@ -1846,7 +1846,7 @@
         <v>1</v>
       </c>
       <c r="D61">
-        <f t="shared" si="3"/>
+        <f>IF(B61=C61,1,0)</f>
         <v>1</v>
       </c>
       <c r="E61">
@@ -1855,16 +1855,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B62" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D62">
-        <f t="shared" si="3"/>
+        <f>IF(B62=C62,1,0)</f>
         <v>1</v>
       </c>
       <c r="E62">
@@ -1873,16 +1873,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D63">
-        <f t="shared" si="3"/>
+        <f>IF(B63=C63,1,0)</f>
         <v>1</v>
       </c>
       <c r="E63">
@@ -1891,17 +1891,17 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D64">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(B64=C64,1,0)</f>
+        <v>1</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -1909,16 +1909,16 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B65" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D65">
-        <f t="shared" si="3"/>
+        <f>IF(B65=C65,1,0)</f>
         <v>1</v>
       </c>
       <c r="E65">
@@ -1927,17 +1927,17 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D68" si="6">IF(B66=C66,1,0)</f>
-        <v>0</v>
+        <f>IF(B66=C66,1,0)</f>
+        <v>1</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -1945,17 +1945,17 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C67" t="s">
         <v>3</v>
       </c>
       <c r="D67">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>IF(B67=C67,1,0)</f>
+        <v>1</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -1972,7 +1972,7 @@
         <v>1</v>
       </c>
       <c r="D68">
-        <f t="shared" si="6"/>
+        <f>IF(B68=C68,1,0)</f>
         <v>1</v>
       </c>
       <c r="E68">
@@ -1996,7 +1996,7 @@
   </sheetData>
   <autoFilter ref="A1:G69">
     <sortState ref="A2:G69">
-      <sortCondition ref="E1:E69"/>
+      <sortCondition ref="D1:D69"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="D1:D1048576 E1">

</xml_diff>

<commit_message>
Like 2.5 sticky notes....
</commit_message>
<xml_diff>
--- a/Relevant Documents/LOOCV_details.xlsx
+++ b/Relevant Documents/LOOCV_details.xlsx
@@ -584,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M69"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +597,7 @@
     <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -614,7 +614,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -625,7 +625,7 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <f>IF(B2=C2,1,0)</f>
+        <f t="shared" ref="D2:D33" si="0">IF(B2=C2,1,0)</f>
         <v>0</v>
       </c>
       <c r="E2">
@@ -639,7 +639,7 @@
         <v>20.689655172413794</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -650,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <f>IF(B3=C3,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E3">
@@ -661,7 +661,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -672,14 +672,14 @@
         <v>5</v>
       </c>
       <c r="D4">
-        <f>IF(B4=C4,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -690,14 +690,14 @@
         <v>21</v>
       </c>
       <c r="D5">
-        <f>IF(B5=C5,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -708,14 +708,14 @@
         <v>21</v>
       </c>
       <c r="D6">
-        <f>IF(B6=C6,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -726,14 +726,14 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <f>IF(B7=C7,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -744,14 +744,18 @@
         <v>3</v>
       </c>
       <c r="D8">
-        <f>IF(B8=C8,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <f>COUNTIF(C:C,K23)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -762,14 +766,14 @@
         <v>3</v>
       </c>
       <c r="D9">
-        <f>IF(B9=C9,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -780,14 +784,14 @@
         <v>21</v>
       </c>
       <c r="D10">
-        <f>IF(B10=C10,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -798,14 +802,14 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <f>IF(B11=C11,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -816,14 +820,14 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <f>IF(B12=C12,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -834,14 +838,14 @@
         <v>3</v>
       </c>
       <c r="D13">
-        <f>IF(B13=C13,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -852,14 +856,14 @@
         <v>3</v>
       </c>
       <c r="D14">
-        <f>IF(B14=C14,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -870,14 +874,14 @@
         <v>5</v>
       </c>
       <c r="D15">
-        <f>IF(B15=C15,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -888,7 +892,7 @@
         <v>3</v>
       </c>
       <c r="D16">
-        <f>IF(B16=C16,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E16">
@@ -906,7 +910,7 @@
         <v>5</v>
       </c>
       <c r="D17">
-        <f>IF(B17=C17,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E17">
@@ -924,7 +928,7 @@
         <v>8</v>
       </c>
       <c r="D18">
-        <f>IF(B18=C18,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E18">
@@ -942,7 +946,7 @@
         <v>8</v>
       </c>
       <c r="D19">
-        <f>IF(B19=C19,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E19">
@@ -960,7 +964,7 @@
         <v>21</v>
       </c>
       <c r="D20">
-        <f>IF(B20=C20,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E20">
@@ -978,7 +982,7 @@
         <v>21</v>
       </c>
       <c r="D21">
-        <f>IF(B21=C21,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E21">
@@ -996,7 +1000,7 @@
         <v>8</v>
       </c>
       <c r="D22">
-        <f>IF(B22=C22,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E22">
@@ -1017,7 +1021,7 @@
         <v>21</v>
       </c>
       <c r="D23">
-        <f>IF(B23=C23,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E23">
@@ -1046,7 +1050,7 @@
         <v>3</v>
       </c>
       <c r="D24">
-        <f>IF(B24=C24,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E24">
@@ -1056,11 +1060,11 @@
         <v>3</v>
       </c>
       <c r="L24">
-        <f t="shared" ref="L24:L27" si="0">COUNTIF(C$2:C$30,K24)</f>
+        <f t="shared" ref="L24:L27" si="1">COUNTIF(C$2:C$30,K24)</f>
         <v>8</v>
       </c>
       <c r="M24">
-        <f t="shared" ref="M24:M28" si="1">L24/$L$29*100</f>
+        <f t="shared" ref="M24:M28" si="2">L24/$L$29*100</f>
         <v>26.666666666666668</v>
       </c>
     </row>
@@ -1075,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="D25">
-        <f>IF(B25=C25,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E25">
@@ -1088,11 +1092,11 @@
         <v>5</v>
       </c>
       <c r="L25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="M25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16.666666666666664</v>
       </c>
     </row>
@@ -1107,7 +1111,7 @@
         <v>8</v>
       </c>
       <c r="D26">
-        <f>IF(B26=C26,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E26">
@@ -1117,11 +1121,11 @@
         <v>21</v>
       </c>
       <c r="L26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="M26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
@@ -1136,7 +1140,7 @@
         <v>1</v>
       </c>
       <c r="D27">
-        <f>IF(B27=C27,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E27">
@@ -1146,11 +1150,11 @@
         <v>8</v>
       </c>
       <c r="L27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="M27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.333333333333334</v>
       </c>
     </row>
@@ -1165,7 +1169,7 @@
         <v>5</v>
       </c>
       <c r="D28">
-        <f>IF(B28=C28,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E28">
@@ -1178,7 +1182,7 @@
         <v>1</v>
       </c>
       <c r="M28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.3333333333333335</v>
       </c>
     </row>
@@ -1193,7 +1197,7 @@
         <v>3</v>
       </c>
       <c r="D29">
-        <f>IF(B29=C29,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E29">
@@ -1215,7 +1219,7 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <f>IF(B30=C30,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E30">
@@ -1233,7 +1237,7 @@
         <v>3</v>
       </c>
       <c r="D31">
-        <f>IF(B31=C31,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E31">
@@ -1251,7 +1255,7 @@
         <v>3</v>
       </c>
       <c r="D32">
-        <f>IF(B32=C32,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E32">
@@ -1269,7 +1273,7 @@
         <v>1</v>
       </c>
       <c r="D33">
-        <f>IF(B33=C33,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E33">
@@ -1287,7 +1291,7 @@
         <v>21</v>
       </c>
       <c r="D34">
-        <f>IF(B34=C34,1,0)</f>
+        <f t="shared" ref="D34:D65" si="3">IF(B34=C34,1,0)</f>
         <v>1</v>
       </c>
       <c r="E34">
@@ -1305,7 +1309,7 @@
         <v>1</v>
       </c>
       <c r="D35">
-        <f>IF(B35=C35,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E35">
@@ -1326,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="D36">
-        <f>IF(B36=C36,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E36">
@@ -1355,7 +1359,7 @@
         <v>5</v>
       </c>
       <c r="D37">
-        <f>IF(B37=C37,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E37">
@@ -1365,11 +1369,11 @@
         <v>3</v>
       </c>
       <c r="L37">
-        <f t="shared" ref="L37:L40" si="2">COUNTIF(C$31:C$68,K37)</f>
+        <f t="shared" ref="L37:L40" si="4">COUNTIF(C$31:C$68,K37)</f>
         <v>9</v>
       </c>
       <c r="M37">
-        <f t="shared" ref="M37:M41" si="3">L37/$L$42*100</f>
+        <f t="shared" ref="M37:M41" si="5">L37/$L$42*100</f>
         <v>23.076923076923077</v>
       </c>
     </row>
@@ -1384,7 +1388,7 @@
         <v>8</v>
       </c>
       <c r="D38">
-        <f>IF(B38=C38,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E38">
@@ -1394,11 +1398,11 @@
         <v>5</v>
       </c>
       <c r="L38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="M38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7.6923076923076925</v>
       </c>
     </row>
@@ -1413,7 +1417,7 @@
         <v>5</v>
       </c>
       <c r="D39">
-        <f>IF(B39=C39,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E39">
@@ -1423,11 +1427,11 @@
         <v>21</v>
       </c>
       <c r="L39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.5641025641025639</v>
       </c>
     </row>
@@ -1442,7 +1446,7 @@
         <v>3</v>
       </c>
       <c r="D40">
-        <f>IF(B40=C40,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E40">
@@ -1452,11 +1456,11 @@
         <v>8</v>
       </c>
       <c r="L40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.5641025641025639</v>
       </c>
     </row>
@@ -1471,7 +1475,7 @@
         <v>1</v>
       </c>
       <c r="D41">
-        <f>IF(B41=C41,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E41">
@@ -1485,7 +1489,7 @@
         <v>1</v>
       </c>
       <c r="M41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.5641025641025639</v>
       </c>
     </row>
@@ -1500,7 +1504,7 @@
         <v>3</v>
       </c>
       <c r="D42">
-        <f>IF(B42=C42,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E42">
@@ -1522,7 +1526,7 @@
         <v>1</v>
       </c>
       <c r="D43">
-        <f>IF(B43=C43,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E43">
@@ -1540,7 +1544,7 @@
         <v>1</v>
       </c>
       <c r="D44">
-        <f>IF(B44=C44,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E44">
@@ -1558,7 +1562,7 @@
         <v>1</v>
       </c>
       <c r="D45">
-        <f>IF(B45=C45,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E45">
@@ -1576,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="D46">
-        <f>IF(B46=C46,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E46">
@@ -1594,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="D47">
-        <f>IF(B47=C47,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E47">
@@ -1612,7 +1616,7 @@
         <v>1</v>
       </c>
       <c r="D48">
-        <f>IF(B48=C48,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E48">
@@ -1630,7 +1634,7 @@
         <v>1</v>
       </c>
       <c r="D49">
-        <f>IF(B49=C49,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E49">
@@ -1648,7 +1652,7 @@
         <v>1</v>
       </c>
       <c r="D50">
-        <f>IF(B50=C50,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E50">
@@ -1666,7 +1670,7 @@
         <v>1</v>
       </c>
       <c r="D51">
-        <f>IF(B51=C51,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E51">
@@ -1684,7 +1688,7 @@
         <v>3</v>
       </c>
       <c r="D52">
-        <f>IF(B52=C52,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E52">
@@ -1702,7 +1706,7 @@
         <v>1</v>
       </c>
       <c r="D53">
-        <f>IF(B53=C53,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E53">
@@ -1720,7 +1724,7 @@
         <v>1</v>
       </c>
       <c r="D54">
-        <f>IF(B54=C54,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E54">
@@ -1738,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="D55">
-        <f>IF(B55=C55,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E55">
@@ -1756,7 +1760,7 @@
         <v>1</v>
       </c>
       <c r="D56">
-        <f>IF(B56=C56,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E56">
@@ -1774,7 +1778,7 @@
         <v>3</v>
       </c>
       <c r="D57">
-        <f>IF(B57=C57,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E57">
@@ -1792,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="D58">
-        <f>IF(B58=C58,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E58">
@@ -1810,7 +1814,7 @@
         <v>1</v>
       </c>
       <c r="D59">
-        <f>IF(B59=C59,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E59">
@@ -1828,7 +1832,7 @@
         <v>3</v>
       </c>
       <c r="D60">
-        <f>IF(B60=C60,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E60">
@@ -1846,7 +1850,7 @@
         <v>1</v>
       </c>
       <c r="D61">
-        <f>IF(B61=C61,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E61">
@@ -1864,7 +1868,7 @@
         <v>3</v>
       </c>
       <c r="D62">
-        <f>IF(B62=C62,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E62">
@@ -1882,7 +1886,7 @@
         <v>1</v>
       </c>
       <c r="D63">
-        <f>IF(B63=C63,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E63">
@@ -1900,7 +1904,7 @@
         <v>1</v>
       </c>
       <c r="D64">
-        <f>IF(B64=C64,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E64">
@@ -1918,7 +1922,7 @@
         <v>1</v>
       </c>
       <c r="D65">
-        <f>IF(B65=C65,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E65">
@@ -1936,7 +1940,7 @@
         <v>5</v>
       </c>
       <c r="D66">
-        <f>IF(B66=C66,1,0)</f>
+        <f t="shared" ref="D66:D97" si="6">IF(B66=C66,1,0)</f>
         <v>1</v>
       </c>
       <c r="E66">
@@ -1954,7 +1958,7 @@
         <v>3</v>
       </c>
       <c r="D67">
-        <f>IF(B67=C67,1,0)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E67">
@@ -1972,7 +1976,7 @@
         <v>1</v>
       </c>
       <c r="D68">
-        <f>IF(B68=C68,1,0)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E68">

</xml_diff>